<commit_message>
Numbers good, need structure still
</commit_message>
<xml_diff>
--- a/data_work_example.xlsx
+++ b/data_work_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshatdhir/Repositories/pectus_data_transform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAD218D-1185-5449-8A79-05F9B72E5453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F81139-E7CC-DE47-BCA0-BF40D97D9923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{669C2DF5-7C29-8346-9A88-211B85899BEB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15560" xr2:uid="{669C2DF5-7C29-8346-9A88-211B85899BEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>Level 1 List Order</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>Zugang Immat.Verm.</t>
+  </si>
+  <si>
+    <t>Ausz.SAV-Invest.</t>
+  </si>
+  <si>
+    <t>Zugang Sachanlagen</t>
+  </si>
+  <si>
+    <t>Einz.kfr.Finanzdisp. L1</t>
+  </si>
+  <si>
+    <t>Einz.kfr.Finanzdisp.</t>
   </si>
 </sst>
 </file>
@@ -437,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E068004-25AA-514E-A54F-29AD2345CE8C}">
-  <dimension ref="A1:AZ8"/>
+  <dimension ref="A1:AZ19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1575,188 +1587,1880 @@
         <v>3510</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ref="G8:AZ8" si="0">G7*0.89</f>
         <v>-9.0827220684353076</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="0"/>
         <v>-6.3985537147913734</v>
       </c>
       <c r="I8" s="3">
-        <f t="shared" si="0"/>
         <v>-9.5668462073223068</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="0"/>
         <v>-11.820459632042594</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="0"/>
         <v>-18.564208156133805</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="0"/>
         <v>-15.923876387087752</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" si="0"/>
         <v>-21.825318523717307</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" si="0"/>
         <v>-16.25800864705916</v>
       </c>
       <c r="O8" s="3">
-        <f t="shared" si="0"/>
         <v>-27.91635436597819</v>
       </c>
       <c r="P8" s="3">
-        <f t="shared" si="0"/>
         <v>-51.608001638833109</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" si="0"/>
         <v>-27.91635436597819</v>
       </c>
       <c r="R8" s="3">
-        <f t="shared" si="0"/>
         <v>-51.608001638833109</v>
       </c>
       <c r="S8" s="3">
-        <f t="shared" si="0"/>
         <v>-9.0827220684353076</v>
       </c>
       <c r="T8" s="3">
-        <f t="shared" si="0"/>
         <v>-6.3985537147913734</v>
       </c>
       <c r="U8" s="3">
-        <f t="shared" si="0"/>
         <v>-9.5668462073223068</v>
       </c>
       <c r="V8" s="3">
-        <f t="shared" si="0"/>
         <v>-11.820459632042594</v>
       </c>
       <c r="W8" s="3">
-        <f t="shared" si="0"/>
         <v>-18.564208156133805</v>
       </c>
       <c r="X8" s="3">
-        <f t="shared" si="0"/>
         <v>-15.923876387087752</v>
       </c>
       <c r="Y8" s="3">
-        <f t="shared" si="0"/>
         <v>-21.825318523717307</v>
       </c>
       <c r="Z8" s="3">
-        <f t="shared" si="0"/>
         <v>-16.25800864705916</v>
       </c>
       <c r="AA8" s="3">
-        <f t="shared" si="0"/>
         <v>-27.91635436597819</v>
       </c>
       <c r="AB8" s="3">
-        <f t="shared" si="0"/>
         <v>-51.608001638833109</v>
       </c>
       <c r="AC8" s="3">
-        <f t="shared" si="0"/>
         <v>-48.409356336237963</v>
       </c>
       <c r="AD8" s="3">
-        <f t="shared" si="0"/>
         <v>-48.051514522744746</v>
       </c>
       <c r="AE8" s="3">
-        <f t="shared" si="0"/>
         <v>-50.033941179559548</v>
       </c>
       <c r="AF8" s="3">
-        <f t="shared" si="0"/>
         <v>-34.231059238376425</v>
       </c>
       <c r="AG8" s="3">
-        <f t="shared" si="0"/>
         <v>-33.520132157621155</v>
       </c>
       <c r="AH8" s="3">
-        <f t="shared" si="0"/>
         <v>-31.1208188813204</v>
       </c>
       <c r="AI8" s="3">
-        <f t="shared" si="0"/>
         <v>-45.552052881413609</v>
       </c>
       <c r="AJ8" s="3">
-        <f t="shared" si="0"/>
         <v>-38.593413461668</v>
       </c>
       <c r="AK8" s="3">
-        <f t="shared" si="0"/>
         <v>-21.227737235261369</v>
       </c>
       <c r="AL8" s="3">
-        <f t="shared" si="0"/>
         <v>-39.300968007971676</v>
       </c>
       <c r="AM8" s="3">
-        <f t="shared" si="0"/>
         <v>-35.535969176960478</v>
       </c>
       <c r="AN8" s="3">
-        <f t="shared" si="0"/>
         <v>-129.2581829794525</v>
       </c>
       <c r="AO8" s="3">
-        <f t="shared" si="0"/>
         <v>-43.847249442688749</v>
       </c>
       <c r="AP8" s="3">
-        <f t="shared" si="0"/>
         <v>-37.958941100602686</v>
       </c>
       <c r="AQ8" s="3">
-        <f t="shared" si="0"/>
         <v>-32.513322448193371</v>
       </c>
       <c r="AR8" s="3">
-        <f t="shared" si="0"/>
         <v>-19.995053621757638</v>
       </c>
       <c r="AS8" s="3">
-        <f t="shared" si="0"/>
         <v>-55.55981024373493</v>
       </c>
       <c r="AT8" s="3">
-        <f t="shared" si="0"/>
         <v>-56.896030664902</v>
       </c>
       <c r="AU8" s="3">
-        <f t="shared" si="0"/>
         <v>-64.030675021748038</v>
       </c>
       <c r="AV8" s="3">
-        <f t="shared" si="0"/>
         <v>-65.446859507416377</v>
       </c>
       <c r="AW8" s="3">
-        <f t="shared" si="0"/>
         <v>-66.713440273794745</v>
       </c>
       <c r="AX8" s="3">
-        <f t="shared" si="0"/>
         <v>-71.084244923032884</v>
       </c>
       <c r="AY8" s="3">
-        <f t="shared" si="0"/>
         <v>-68.419322287216829</v>
       </c>
       <c r="AZ8" s="3">
-        <f t="shared" si="0"/>
         <v>-89.339395294679136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>5923</v>
+      </c>
+      <c r="F9">
+        <v>3510</v>
+      </c>
+      <c r="G9" s="3">
+        <v>-8.0836226409074232</v>
+      </c>
+      <c r="H9" s="3">
+        <v>-5.694712806164322</v>
+      </c>
+      <c r="I9" s="3">
+        <v>-8.5144931245168536</v>
+      </c>
+      <c r="J9" s="3">
+        <v>-10.520209072517909</v>
+      </c>
+      <c r="K9" s="3">
+        <v>-16.522145258959085</v>
+      </c>
+      <c r="L9" s="3">
+        <v>-14.172249984508099</v>
+      </c>
+      <c r="M9" s="3">
+        <v>-19.424533486108405</v>
+      </c>
+      <c r="N9" s="3">
+        <v>-14.469627695882654</v>
+      </c>
+      <c r="O9" s="3">
+        <v>-24.845555385720591</v>
+      </c>
+      <c r="P9" s="3">
+        <v>-45.931121458561471</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>-24.845555385720591</v>
+      </c>
+      <c r="R9" s="3">
+        <v>-45.931121458561471</v>
+      </c>
+      <c r="S9" s="3">
+        <v>-8.0836226409074232</v>
+      </c>
+      <c r="T9" s="3">
+        <v>-5.694712806164322</v>
+      </c>
+      <c r="U9" s="3">
+        <v>-8.5144931245168536</v>
+      </c>
+      <c r="V9" s="3">
+        <v>-10.520209072517909</v>
+      </c>
+      <c r="W9" s="3">
+        <v>-16.522145258959085</v>
+      </c>
+      <c r="X9" s="3">
+        <v>-14.172249984508099</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>-19.424533486108405</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>-14.469627695882654</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>-24.845555385720591</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>-45.931121458561471</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>-43.084327139251791</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>-42.765847925242824</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>-44.530207649807998</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>-30.465642722155017</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>-29.832917620282828</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>-27.697528804375157</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>-40.541327064458109</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>-34.348137980884523</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>-18.892686139382619</v>
+      </c>
+      <c r="AL9" s="3">
+        <v>-34.977861527094795</v>
+      </c>
+      <c r="AM9" s="3">
+        <v>-31.627012567494827</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>-115.03978285171273</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>-39.024052003992985</v>
+      </c>
+      <c r="AP9" s="3">
+        <v>-33.783457579536389</v>
+      </c>
+      <c r="AQ9" s="3">
+        <v>-28.936856978892102</v>
+      </c>
+      <c r="AR9" s="3">
+        <v>-17.795597723364299</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>-49.448231116924092</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>-50.637467291762782</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>-56.987300769355755</v>
+      </c>
+      <c r="AV9" s="3">
+        <v>-58.247704961600576</v>
+      </c>
+      <c r="AW9" s="3">
+        <v>-59.374961843677326</v>
+      </c>
+      <c r="AX9" s="3">
+        <v>-63.264977981499264</v>
+      </c>
+      <c r="AY9" s="3">
+        <v>-60.89319683562298</v>
+      </c>
+      <c r="AZ9" s="3">
+        <v>-79.512061812264434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>6811</v>
+      </c>
+      <c r="F10">
+        <v>3510</v>
+      </c>
+      <c r="G10" s="3">
+        <v>-7.194424150407607</v>
+      </c>
+      <c r="H10" s="3">
+        <v>-5.0682943974862464</v>
+      </c>
+      <c r="I10" s="3">
+        <v>-7.5778988808199994</v>
+      </c>
+      <c r="J10" s="3">
+        <v>-9.3629860745409399</v>
+      </c>
+      <c r="K10" s="3">
+        <v>-14.704709280473587</v>
+      </c>
+      <c r="L10" s="3">
+        <v>-12.613302486212207</v>
+      </c>
+      <c r="M10" s="3">
+        <v>-17.287834802636482</v>
+      </c>
+      <c r="N10" s="3">
+        <v>-12.877968649335562</v>
+      </c>
+      <c r="O10" s="3">
+        <v>-22.112544293291325</v>
+      </c>
+      <c r="P10" s="3">
+        <v>-40.878698098119706</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>-22.112544293291325</v>
+      </c>
+      <c r="R10" s="3">
+        <v>-40.878698098119706</v>
+      </c>
+      <c r="S10" s="3">
+        <v>-7.194424150407607</v>
+      </c>
+      <c r="T10" s="3">
+        <v>-5.0682943974862464</v>
+      </c>
+      <c r="U10" s="3">
+        <v>-7.5778988808199994</v>
+      </c>
+      <c r="V10" s="3">
+        <v>-9.3629860745409399</v>
+      </c>
+      <c r="W10" s="3">
+        <v>-14.704709280473587</v>
+      </c>
+      <c r="X10" s="3">
+        <v>-12.613302486212207</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>-17.287834802636482</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>-12.877968649335562</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>-22.112544293291325</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>-40.878698098119706</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>-38.345051153934094</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>-38.061604653466112</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>-39.631884808329119</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>-27.114422022717967</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>-26.551296682051717</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>-24.650800635893891</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>-36.081781087367716</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>-30.569842802987225</v>
+      </c>
+      <c r="AK10" s="3">
+        <v>-16.814490664050531</v>
+      </c>
+      <c r="AL10" s="3">
+        <v>-31.130296759114369</v>
+      </c>
+      <c r="AM10" s="3">
+        <v>-28.148041185070397</v>
+      </c>
+      <c r="AN10" s="3">
+        <v>-102.38540673802433</v>
+      </c>
+      <c r="AO10" s="3">
+        <v>-34.73140628355376</v>
+      </c>
+      <c r="AP10" s="3">
+        <v>-30.067277245787388</v>
+      </c>
+      <c r="AQ10" s="3">
+        <v>-25.753802711213972</v>
+      </c>
+      <c r="AR10" s="3">
+        <v>-15.838081973794226</v>
+      </c>
+      <c r="AS10" s="3">
+        <v>-44.008925694062441</v>
+      </c>
+      <c r="AT10" s="3">
+        <v>-45.067345889668879</v>
+      </c>
+      <c r="AU10" s="3">
+        <v>-50.718697684726621</v>
+      </c>
+      <c r="AV10" s="3">
+        <v>-51.84045741582451</v>
+      </c>
+      <c r="AW10" s="3">
+        <v>-52.84371604087282</v>
+      </c>
+      <c r="AX10" s="3">
+        <v>-56.305830403534344</v>
+      </c>
+      <c r="AY10" s="3">
+        <v>-54.194945183704455</v>
+      </c>
+      <c r="AZ10" s="3">
+        <v>-70.765735012915343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>6811</v>
+      </c>
+      <c r="F11">
+        <v>71700</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-6.4030374938627705</v>
+      </c>
+      <c r="H11" s="3">
+        <v>-4.5107820137627597</v>
+      </c>
+      <c r="I11" s="3">
+        <v>-6.7443300039297993</v>
+      </c>
+      <c r="J11" s="3">
+        <v>-8.3330576063414359</v>
+      </c>
+      <c r="K11" s="3">
+        <v>-13.087191259621493</v>
+      </c>
+      <c r="L11" s="3">
+        <v>-11.225839212728864</v>
+      </c>
+      <c r="M11" s="3">
+        <v>-15.386172974346469</v>
+      </c>
+      <c r="N11" s="3">
+        <v>-11.46139209790865</v>
+      </c>
+      <c r="O11" s="3">
+        <v>-19.680164421029279</v>
+      </c>
+      <c r="P11" s="3">
+        <v>-36.382041307326539</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>-19.680164421029279</v>
+      </c>
+      <c r="R11" s="3">
+        <v>-36.382041307326539</v>
+      </c>
+      <c r="S11" s="3">
+        <v>-6.4030374938627705</v>
+      </c>
+      <c r="T11" s="3">
+        <v>-4.5107820137627597</v>
+      </c>
+      <c r="U11" s="3">
+        <v>-6.7443300039297993</v>
+      </c>
+      <c r="V11" s="3">
+        <v>-8.3330576063414359</v>
+      </c>
+      <c r="W11" s="3">
+        <v>-13.087191259621493</v>
+      </c>
+      <c r="X11" s="3">
+        <v>-11.225839212728864</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>-15.386172974346469</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>-11.46139209790865</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>-19.680164421029279</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>-36.382041307326539</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>-34.127095527001345</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>-33.874828141584842</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>-35.272377479412917</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>-24.131835600218992</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>-23.630654047026027</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>-21.939212565945564</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>-32.112785167757266</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>-27.207160094658629</v>
+      </c>
+      <c r="AK11" s="3">
+        <v>-14.964896691004974</v>
+      </c>
+      <c r="AL11" s="3">
+        <v>-27.705964115611788</v>
+      </c>
+      <c r="AM11" s="3">
+        <v>-25.051756654712655</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>-91.123011996841655</v>
+      </c>
+      <c r="AO11" s="3">
+        <v>-30.910951592362846</v>
+      </c>
+      <c r="AP11" s="3">
+        <v>-26.759876748750774</v>
+      </c>
+      <c r="AQ11" s="3">
+        <v>-22.920884412980435</v>
+      </c>
+      <c r="AR11" s="3">
+        <v>-14.095892956676861</v>
+      </c>
+      <c r="AS11" s="3">
+        <v>-39.167943867715572</v>
+      </c>
+      <c r="AT11" s="3">
+        <v>-40.109937841805305</v>
+      </c>
+      <c r="AU11" s="3">
+        <v>-45.139640939406696</v>
+      </c>
+      <c r="AV11" s="3">
+        <v>-46.138007100083811</v>
+      </c>
+      <c r="AW11" s="3">
+        <v>-47.030907276376809</v>
+      </c>
+      <c r="AX11" s="3">
+        <v>-50.112189059145564</v>
+      </c>
+      <c r="AY11" s="3">
+        <v>-48.233501213496965</v>
+      </c>
+      <c r="AZ11" s="3">
+        <v>-62.981504161494655</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>6811</v>
+      </c>
+      <c r="F12">
+        <v>71100</v>
+      </c>
+      <c r="G12" s="3">
+        <v>-5.6987033695378662</v>
+      </c>
+      <c r="H12" s="3">
+        <v>-4.0145959922488563</v>
+      </c>
+      <c r="I12" s="3">
+        <v>-6.0024537034975216</v>
+      </c>
+      <c r="J12" s="3">
+        <v>-7.4164212696438785</v>
+      </c>
+      <c r="K12" s="3">
+        <v>-11.647600221063129</v>
+      </c>
+      <c r="L12" s="3">
+        <v>-9.9909968993286888</v>
+      </c>
+      <c r="M12" s="3">
+        <v>-13.693693947168358</v>
+      </c>
+      <c r="N12" s="3">
+        <v>-10.200638967138699</v>
+      </c>
+      <c r="O12" s="3">
+        <v>-17.515346334716057</v>
+      </c>
+      <c r="P12" s="3">
+        <v>-32.380016763520622</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>-17.515346334716057</v>
+      </c>
+      <c r="R12" s="3">
+        <v>-32.380016763520622</v>
+      </c>
+      <c r="S12" s="3">
+        <v>-5.6987033695378662</v>
+      </c>
+      <c r="T12" s="3">
+        <v>-4.0145959922488563</v>
+      </c>
+      <c r="U12" s="3">
+        <v>-6.0024537034975216</v>
+      </c>
+      <c r="V12" s="3">
+        <v>-7.4164212696438785</v>
+      </c>
+      <c r="W12" s="3">
+        <v>-11.647600221063129</v>
+      </c>
+      <c r="X12" s="3">
+        <v>-9.9909968993286888</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>-13.693693947168358</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>-10.200638967138699</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>-17.515346334716057</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>-32.380016763520622</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>-30.373115019031196</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>-30.148597046010511</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>-31.392415956677496</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>-21.477333684194903</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>-21.031282101853165</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>-19.525899183691553</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>-28.580378799303968</v>
+      </c>
+      <c r="AJ12" s="3">
+        <v>-24.21437248424618</v>
+      </c>
+      <c r="AK12" s="3">
+        <v>-13.318758054994428</v>
+      </c>
+      <c r="AL12" s="3">
+        <v>-24.658308062894491</v>
+      </c>
+      <c r="AM12" s="3">
+        <v>-22.296063422694264</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>-81.099480677189078</v>
+      </c>
+      <c r="AO12" s="3">
+        <v>-27.510746917202933</v>
+      </c>
+      <c r="AP12" s="3">
+        <v>-23.81629030638819</v>
+      </c>
+      <c r="AQ12" s="3">
+        <v>-20.399587127552586</v>
+      </c>
+      <c r="AR12" s="3">
+        <v>-12.545344731442407</v>
+      </c>
+      <c r="AS12" s="3">
+        <v>-34.859470042266857</v>
+      </c>
+      <c r="AT12" s="3">
+        <v>-35.697844679206725</v>
+      </c>
+      <c r="AU12" s="3">
+        <v>-40.17428043607196</v>
+      </c>
+      <c r="AV12" s="3">
+        <v>-41.062826319074595</v>
+      </c>
+      <c r="AW12" s="3">
+        <v>-41.85750747597536</v>
+      </c>
+      <c r="AX12" s="3">
+        <v>-44.599848262639554</v>
+      </c>
+      <c r="AY12" s="3">
+        <v>-42.927816080012299</v>
+      </c>
+      <c r="AZ12" s="3">
+        <v>-56.053538703730247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>6837</v>
+      </c>
+      <c r="F13">
+        <v>3510</v>
+      </c>
+      <c r="G13" s="3">
+        <v>-5.0718459988887012</v>
+      </c>
+      <c r="H13" s="3">
+        <v>-3.5729904331014821</v>
+      </c>
+      <c r="I13" s="3">
+        <v>-5.3421837961127947</v>
+      </c>
+      <c r="J13" s="3">
+        <v>-6.6006149299830517</v>
+      </c>
+      <c r="K13" s="3">
+        <v>-10.366364196746185</v>
+      </c>
+      <c r="L13" s="3">
+        <v>-8.8919872404025337</v>
+      </c>
+      <c r="M13" s="3">
+        <v>-12.187387612979839</v>
+      </c>
+      <c r="N13" s="3">
+        <v>-9.0785686807534418</v>
+      </c>
+      <c r="O13" s="3">
+        <v>-15.58865823789729</v>
+      </c>
+      <c r="P13" s="3">
+        <v>-28.818214919533354</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>-15.58865823789729</v>
+      </c>
+      <c r="R13" s="3">
+        <v>-28.818214919533354</v>
+      </c>
+      <c r="S13" s="3">
+        <v>-5.0718459988887012</v>
+      </c>
+      <c r="T13" s="3">
+        <v>-3.5729904331014821</v>
+      </c>
+      <c r="U13" s="3">
+        <v>-5.3421837961127947</v>
+      </c>
+      <c r="V13" s="3">
+        <v>-6.6006149299830517</v>
+      </c>
+      <c r="W13" s="3">
+        <v>-10.366364196746185</v>
+      </c>
+      <c r="X13" s="3">
+        <v>-8.8919872404025337</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>-12.187387612979839</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>-9.0785686807534418</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>-15.58865823789729</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>-28.818214919533354</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>-27.032072366937765</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>-26.832251370949354</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>-27.93925020144297</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>-19.114826978933465</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>-18.717841070649317</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>-17.378050273485481</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>-25.436537131380533</v>
+      </c>
+      <c r="AJ13" s="3">
+        <v>-21.550791510979099</v>
+      </c>
+      <c r="AK13" s="3">
+        <v>-11.853694668945041</v>
+      </c>
+      <c r="AL13" s="3">
+        <v>-21.945894175976097</v>
+      </c>
+      <c r="AM13" s="3">
+        <v>-19.843496446197896</v>
+      </c>
+      <c r="AN13" s="3">
+        <v>-72.178537802698287</v>
+      </c>
+      <c r="AO13" s="3">
+        <v>-24.484564756310611</v>
+      </c>
+      <c r="AP13" s="3">
+        <v>-21.19649837268549</v>
+      </c>
+      <c r="AQ13" s="3">
+        <v>-18.155632543521801</v>
+      </c>
+      <c r="AR13" s="3">
+        <v>-11.165356810983743</v>
+      </c>
+      <c r="AS13" s="3">
+        <v>-31.024928337617503</v>
+      </c>
+      <c r="AT13" s="3">
+        <v>-31.771081764493985</v>
+      </c>
+      <c r="AU13" s="3">
+        <v>-35.755109588104048</v>
+      </c>
+      <c r="AV13" s="3">
+        <v>-36.545915423976389</v>
+      </c>
+      <c r="AW13" s="3">
+        <v>-37.253181653618071</v>
+      </c>
+      <c r="AX13" s="3">
+        <v>-39.693864953749205</v>
+      </c>
+      <c r="AY13" s="3">
+        <v>-38.205756311210948</v>
+      </c>
+      <c r="AZ13" s="3">
+        <v>-49.887649446319919</v>
+      </c>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>6851</v>
+      </c>
+      <c r="F14">
+        <v>1420</v>
+      </c>
+      <c r="G14" s="3">
+        <v>-4.5139429390109438</v>
+      </c>
+      <c r="H14" s="3">
+        <v>-3.1799614854603191</v>
+      </c>
+      <c r="I14" s="3">
+        <v>-4.7545435785403871</v>
+      </c>
+      <c r="J14" s="3">
+        <v>-5.8745472876849156</v>
+      </c>
+      <c r="K14" s="3">
+        <v>-9.2260641351041048</v>
+      </c>
+      <c r="L14" s="3">
+        <v>-7.9138686439582555</v>
+      </c>
+      <c r="M14" s="3">
+        <v>-10.846774975552057</v>
+      </c>
+      <c r="N14" s="3">
+        <v>-8.0799261258705641</v>
+      </c>
+      <c r="O14" s="3">
+        <v>-13.873905831728589</v>
+      </c>
+      <c r="P14" s="3">
+        <v>-25.648211278384686</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>-13.873905831728589</v>
+      </c>
+      <c r="R14" s="3">
+        <v>-25.648211278384686</v>
+      </c>
+      <c r="S14" s="3">
+        <v>-4.5139429390109438</v>
+      </c>
+      <c r="T14" s="3">
+        <v>-3.1799614854603191</v>
+      </c>
+      <c r="U14" s="3">
+        <v>-4.7545435785403871</v>
+      </c>
+      <c r="V14" s="3">
+        <v>-5.8745472876849156</v>
+      </c>
+      <c r="W14" s="3">
+        <v>-9.2260641351041048</v>
+      </c>
+      <c r="X14" s="3">
+        <v>-7.9138686439582555</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>-10.846774975552057</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>-8.0799261258705641</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>-13.873905831728589</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>-25.648211278384686</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>-24.058544406574612</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>-23.880703720144925</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>-24.865932679284242</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>-17.012196011250783</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>-16.658878552877894</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>-15.466464743402078</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>-22.638518046928674</v>
+      </c>
+      <c r="AJ14" s="3">
+        <v>-19.180204444771398</v>
+      </c>
+      <c r="AK14" s="3">
+        <v>-10.549788255361086</v>
+      </c>
+      <c r="AL14" s="3">
+        <v>-19.531845816618727</v>
+      </c>
+      <c r="AM14" s="3">
+        <v>-17.660711837116128</v>
+      </c>
+      <c r="AN14" s="3">
+        <v>-64.238898644401473</v>
+      </c>
+      <c r="AO14" s="3">
+        <v>-21.791262633116446</v>
+      </c>
+      <c r="AP14" s="3">
+        <v>-18.864883551690085</v>
+      </c>
+      <c r="AQ14" s="3">
+        <v>-16.158512963734402</v>
+      </c>
+      <c r="AR14" s="3">
+        <v>-9.9371675617755315</v>
+      </c>
+      <c r="AS14" s="3">
+        <v>-27.612186220479579</v>
+      </c>
+      <c r="AT14" s="3">
+        <v>-28.276262770399647</v>
+      </c>
+      <c r="AU14" s="3">
+        <v>-31.822047533412604</v>
+      </c>
+      <c r="AV14" s="3">
+        <v>-32.525864727338984</v>
+      </c>
+      <c r="AW14" s="3">
+        <v>-33.155331671720084</v>
+      </c>
+      <c r="AX14" s="3">
+        <v>-35.327539808836796</v>
+      </c>
+      <c r="AY14" s="3">
+        <v>-34.003123116977747</v>
+      </c>
+      <c r="AZ14" s="3">
+        <v>-44.400008007224727</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>6855</v>
+      </c>
+      <c r="F15">
+        <v>71200</v>
+      </c>
+      <c r="G15" s="3">
+        <v>-4.0174092157197396</v>
+      </c>
+      <c r="H15" s="3">
+        <v>-2.8301657220596841</v>
+      </c>
+      <c r="I15" s="3">
+        <v>-4.2315437849009445</v>
+      </c>
+      <c r="J15" s="3">
+        <v>-5.2283470860395749</v>
+      </c>
+      <c r="K15" s="3">
+        <v>-8.2111970802426537</v>
+      </c>
+      <c r="L15" s="3">
+        <v>-7.0433430931228473</v>
+      </c>
+      <c r="M15" s="3">
+        <v>-9.6536297282413308</v>
+      </c>
+      <c r="N15" s="3">
+        <v>-7.1911342520248018</v>
+      </c>
+      <c r="O15" s="3">
+        <v>-12.347776190238445</v>
+      </c>
+      <c r="P15" s="3">
+        <v>-22.826908037762372</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>-12.347776190238445</v>
+      </c>
+      <c r="R15" s="3">
+        <v>-22.826908037762372</v>
+      </c>
+      <c r="S15" s="3">
+        <v>-4.0174092157197396</v>
+      </c>
+      <c r="T15" s="3">
+        <v>-2.8301657220596841</v>
+      </c>
+      <c r="U15" s="3">
+        <v>-4.2315437849009445</v>
+      </c>
+      <c r="V15" s="3">
+        <v>-5.2283470860395749</v>
+      </c>
+      <c r="W15" s="3">
+        <v>-8.2111970802426537</v>
+      </c>
+      <c r="X15" s="3">
+        <v>-7.0433430931228473</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>-9.6536297282413308</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>-7.1911342520248018</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>-12.347776190238445</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>-22.826908037762372</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>-21.412104521851404</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>-21.253826310928982</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>-22.130680084562975</v>
+      </c>
+      <c r="AF15" s="3">
+        <v>-15.140854450013197</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>-14.826401912061327</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>-13.765153621627849</v>
+      </c>
+      <c r="AI15" s="3">
+        <v>-20.148281061766522</v>
+      </c>
+      <c r="AJ15" s="3">
+        <v>-17.070381955846546</v>
+      </c>
+      <c r="AK15" s="3">
+        <v>-9.3893115472713671</v>
+      </c>
+      <c r="AL15" s="3">
+        <v>-17.383342776790666</v>
+      </c>
+      <c r="AM15" s="3">
+        <v>-15.718033535033355</v>
+      </c>
+      <c r="AN15" s="3">
+        <v>-57.172619793517313</v>
+      </c>
+      <c r="AO15" s="3">
+        <v>-19.394223743473638</v>
+      </c>
+      <c r="AP15" s="3">
+        <v>-16.789746361004177</v>
+      </c>
+      <c r="AQ15" s="3">
+        <v>-14.381076537723619</v>
+      </c>
+      <c r="AR15" s="3">
+        <v>-8.8440791299802228</v>
+      </c>
+      <c r="AS15" s="3">
+        <v>-24.574845736226827</v>
+      </c>
+      <c r="AT15" s="3">
+        <v>-25.165873865655687</v>
+      </c>
+      <c r="AU15" s="3">
+        <v>-28.321622304737218</v>
+      </c>
+      <c r="AV15" s="3">
+        <v>-28.948019607331695</v>
+      </c>
+      <c r="AW15" s="3">
+        <v>-29.508245187830877</v>
+      </c>
+      <c r="AX15" s="3">
+        <v>-31.441510429864749</v>
+      </c>
+      <c r="AY15" s="3">
+        <v>-30.262779574110194</v>
+      </c>
+      <c r="AZ15" s="3">
+        <v>-39.516007126430004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16">
+        <v>6880</v>
+      </c>
+      <c r="F16">
+        <v>3510</v>
+      </c>
+      <c r="G16" s="3">
+        <v>-3.5754942019905682</v>
+      </c>
+      <c r="H16" s="3">
+        <v>-2.5188474926331188</v>
+      </c>
+      <c r="I16" s="3">
+        <v>-3.7660739685618405</v>
+      </c>
+      <c r="J16" s="3">
+        <v>-4.6532289065752215</v>
+      </c>
+      <c r="K16" s="3">
+        <v>-7.3079654014159621</v>
+      </c>
+      <c r="L16" s="3">
+        <v>-6.268575352879334</v>
+      </c>
+      <c r="M16" s="3">
+        <v>-8.5917304581347853</v>
+      </c>
+      <c r="N16" s="3">
+        <v>-6.4001094843020736</v>
+      </c>
+      <c r="O16" s="3">
+        <v>-10.989520809312216</v>
+      </c>
+      <c r="P16" s="3">
+        <v>-20.315948153608513</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>-10.989520809312216</v>
+      </c>
+      <c r="R16" s="3">
+        <v>-20.315948153608513</v>
+      </c>
+      <c r="S16" s="3">
+        <v>-3.5754942019905682</v>
+      </c>
+      <c r="T16" s="3">
+        <v>-2.5188474926331188</v>
+      </c>
+      <c r="U16" s="3">
+        <v>-3.7660739685618405</v>
+      </c>
+      <c r="V16" s="3">
+        <v>-4.6532289065752215</v>
+      </c>
+      <c r="W16" s="3">
+        <v>-7.3079654014159621</v>
+      </c>
+      <c r="X16" s="3">
+        <v>-6.268575352879334</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>-8.5917304581347853</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>-6.4001094843020736</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>-10.989520809312216</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>-20.315948153608513</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>-19.05677302444775</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>-18.915905416726794</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>-19.696305275261047</v>
+      </c>
+      <c r="AF16" s="3">
+        <v>-13.475360460511746</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>-13.195497701734581</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>-12.250986723248786</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>-17.931970144972205</v>
+      </c>
+      <c r="AJ16" s="3">
+        <v>-15.192639940703426</v>
+      </c>
+      <c r="AK16" s="3">
+        <v>-8.3564872770715173</v>
+      </c>
+      <c r="AL16" s="3">
+        <v>-15.471175071343692</v>
+      </c>
+      <c r="AM16" s="3">
+        <v>-13.989049846179686</v>
+      </c>
+      <c r="AN16" s="3">
+        <v>-50.88363161623041</v>
+      </c>
+      <c r="AO16" s="3">
+        <v>-17.260859131691539</v>
+      </c>
+      <c r="AP16" s="3">
+        <v>-14.942874261293717</v>
+      </c>
+      <c r="AQ16" s="3">
+        <v>-12.79915811857402</v>
+      </c>
+      <c r="AR16" s="3">
+        <v>-7.8712304256823984</v>
+      </c>
+      <c r="AS16" s="3">
+        <v>-21.871612705241876</v>
+      </c>
+      <c r="AT16" s="3">
+        <v>-22.397627740433563</v>
+      </c>
+      <c r="AU16" s="3">
+        <v>-25.206243851216126</v>
+      </c>
+      <c r="AV16" s="3">
+        <v>-25.763737450525209</v>
+      </c>
+      <c r="AW16" s="3">
+        <v>-26.262338217169482</v>
+      </c>
+      <c r="AX16" s="3">
+        <v>-27.982944282579627</v>
+      </c>
+      <c r="AY16" s="3">
+        <v>-26.933873820958073</v>
+      </c>
+      <c r="AZ16" s="3">
+        <v>-35.169246342522705</v>
+      </c>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>6400</v>
+      </c>
+      <c r="F17">
+        <v>3510</v>
+      </c>
+      <c r="G17" s="3">
+        <v>-3.1821898397716057</v>
+      </c>
+      <c r="H17" s="3">
+        <v>-2.2417742684434758</v>
+      </c>
+      <c r="I17" s="3">
+        <v>-3.3518058320200379</v>
+      </c>
+      <c r="J17" s="3">
+        <v>-4.1413737268519473</v>
+      </c>
+      <c r="K17" s="3">
+        <v>-6.5040892072602059</v>
+      </c>
+      <c r="L17" s="3">
+        <v>-5.5790320640626074</v>
+      </c>
+      <c r="M17" s="3">
+        <v>-7.6466401077399588</v>
+      </c>
+      <c r="N17" s="3">
+        <v>-5.6960974410288454</v>
+      </c>
+      <c r="O17" s="3">
+        <v>-9.7806735202878716</v>
+      </c>
+      <c r="P17" s="3">
+        <v>-18.081193856711575</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>-9.7806735202878716</v>
+      </c>
+      <c r="R17" s="3">
+        <v>-18.081193856711575</v>
+      </c>
+      <c r="S17" s="3">
+        <v>-3.1821898397716057</v>
+      </c>
+      <c r="T17" s="3">
+        <v>-2.2417742684434758</v>
+      </c>
+      <c r="U17" s="3">
+        <v>-3.3518058320200379</v>
+      </c>
+      <c r="V17" s="3">
+        <v>-4.1413737268519473</v>
+      </c>
+      <c r="W17" s="3">
+        <v>-6.5040892072602059</v>
+      </c>
+      <c r="X17" s="3">
+        <v>-5.5790320640626074</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>-7.6466401077399588</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>-5.6960974410288454</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>-9.7806735202878716</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>-18.081193856711575</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>-16.960527991758497</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>-16.835155820886847</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>-17.529711694982332</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>-11.993070809855455</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>-11.743992954543778</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>-10.903378183691419</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>-15.959453429025263</v>
+      </c>
+      <c r="AJ17" s="3">
+        <v>-13.52144954722605</v>
+      </c>
+      <c r="AK17" s="3">
+        <v>-7.4372736765936507</v>
+      </c>
+      <c r="AL17" s="3">
+        <v>-13.769345813495887</v>
+      </c>
+      <c r="AM17" s="3">
+        <v>-12.450254363099921</v>
+      </c>
+      <c r="AN17" s="3">
+        <v>-45.286432138445065</v>
+      </c>
+      <c r="AO17" s="3">
+        <v>-15.36216462720547</v>
+      </c>
+      <c r="AP17" s="3">
+        <v>-13.299158092551409</v>
+      </c>
+      <c r="AQ17" s="3">
+        <v>-11.391250725530877</v>
+      </c>
+      <c r="AR17" s="3">
+        <v>-7.0053950788573349</v>
+      </c>
+      <c r="AS17" s="3">
+        <v>-19.46573530766527</v>
+      </c>
+      <c r="AT17" s="3">
+        <v>-19.933888688985871</v>
+      </c>
+      <c r="AU17" s="3">
+        <v>-22.433557027582353</v>
+      </c>
+      <c r="AV17" s="3">
+        <v>-22.929726330967437</v>
+      </c>
+      <c r="AW17" s="3">
+        <v>-23.373481013280838</v>
+      </c>
+      <c r="AX17" s="3">
+        <v>-24.904820411495869</v>
+      </c>
+      <c r="AY17" s="3">
+        <v>-23.971147700652686</v>
+      </c>
+      <c r="AZ17" s="3">
+        <v>-31.300629244845208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>6420</v>
+      </c>
+      <c r="F18">
+        <v>3510</v>
+      </c>
+      <c r="G18" s="3">
+        <v>-2.8321489573967291</v>
+      </c>
+      <c r="H18" s="3">
+        <v>-1.9951790989146936</v>
+      </c>
+      <c r="I18" s="3">
+        <v>-2.9831071904978339</v>
+      </c>
+      <c r="J18" s="3">
+        <v>-3.6858226168982333</v>
+      </c>
+      <c r="K18" s="3">
+        <v>-5.7886393944615833</v>
+      </c>
+      <c r="L18" s="3">
+        <v>-4.9653385370157208</v>
+      </c>
+      <c r="M18" s="3">
+        <v>-6.8055096958885635</v>
+      </c>
+      <c r="N18" s="3">
+        <v>-5.0695267225156728</v>
+      </c>
+      <c r="O18" s="3">
+        <v>-8.7047994330562055</v>
+      </c>
+      <c r="P18" s="3">
+        <v>-16.092262532473303</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>-8.7047994330562055</v>
+      </c>
+      <c r="R18" s="3">
+        <v>-16.092262532473303</v>
+      </c>
+      <c r="S18" s="3">
+        <v>-2.8321489573967291</v>
+      </c>
+      <c r="T18" s="3">
+        <v>-1.9951790989146936</v>
+      </c>
+      <c r="U18" s="3">
+        <v>-2.9831071904978339</v>
+      </c>
+      <c r="V18" s="3">
+        <v>-3.6858226168982333</v>
+      </c>
+      <c r="W18" s="3">
+        <v>-5.7886393944615833</v>
+      </c>
+      <c r="X18" s="3">
+        <v>-4.9653385370157208</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>-6.8055096958885635</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>-5.0695267225156728</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>-8.7047994330562055</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>-16.092262532473303</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>-15.094869912665063</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>-14.983288680589293</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>-15.601443408534276</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>-10.673833020771355</v>
+      </c>
+      <c r="AG18" s="3">
+        <v>-10.452153729543962</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>-9.7040065834853628</v>
+      </c>
+      <c r="AI18" s="3">
+        <v>-14.203913551832484</v>
+      </c>
+      <c r="AJ18" s="3">
+        <v>-12.034090097031184</v>
+      </c>
+      <c r="AK18" s="3">
+        <v>-6.6191735721683491</v>
+      </c>
+      <c r="AL18" s="3">
+        <v>-12.25471777401134</v>
+      </c>
+      <c r="AM18" s="3">
+        <v>-11.080726383158931</v>
+      </c>
+      <c r="AN18" s="3">
+        <v>-40.304924603216108</v>
+      </c>
+      <c r="AO18" s="3">
+        <v>-13.672326518212868</v>
+      </c>
+      <c r="AP18" s="3">
+        <v>-11.836250702370753</v>
+      </c>
+      <c r="AQ18" s="3">
+        <v>-10.138213145722482</v>
+      </c>
+      <c r="AR18" s="3">
+        <v>-6.2348016201830285</v>
+      </c>
+      <c r="AS18" s="3">
+        <v>-17.324504423822091</v>
+      </c>
+      <c r="AT18" s="3">
+        <v>-17.741160933197424</v>
+      </c>
+      <c r="AU18" s="3">
+        <v>-19.965865754548293</v>
+      </c>
+      <c r="AV18" s="3">
+        <v>-20.40745643456102</v>
+      </c>
+      <c r="AW18" s="3">
+        <v>-20.802398101819946</v>
+      </c>
+      <c r="AX18" s="3">
+        <v>-22.165290166231323</v>
+      </c>
+      <c r="AY18" s="3">
+        <v>-21.334321453580891</v>
+      </c>
+      <c r="AZ18" s="3">
+        <v>-27.857560027912236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>6430</v>
+      </c>
+      <c r="F19">
+        <v>3510</v>
+      </c>
+      <c r="G19" s="3">
+        <v>-2.5206125720830888</v>
+      </c>
+      <c r="H19" s="3">
+        <v>-1.7757093980340772</v>
+      </c>
+      <c r="I19" s="3">
+        <v>-2.6549653995430722</v>
+      </c>
+      <c r="J19" s="3">
+        <v>-3.2803821290394275</v>
+      </c>
+      <c r="K19" s="3">
+        <v>-5.1518890610708095</v>
+      </c>
+      <c r="L19" s="3">
+        <v>-4.4191512979439915</v>
+      </c>
+      <c r="M19" s="3">
+        <v>-6.0569036293408214</v>
+      </c>
+      <c r="N19" s="3">
+        <v>-4.5118787830389486</v>
+      </c>
+      <c r="O19" s="3">
+        <v>-7.7472714954200228</v>
+      </c>
+      <c r="P19" s="3">
+        <v>-14.322113653901239</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>-7.7472714954200228</v>
+      </c>
+      <c r="R19" s="3">
+        <v>-14.322113653901239</v>
+      </c>
+      <c r="S19" s="3">
+        <v>-2.5206125720830888</v>
+      </c>
+      <c r="T19" s="3">
+        <v>-1.7757093980340772</v>
+      </c>
+      <c r="U19" s="3">
+        <v>-2.6549653995430722</v>
+      </c>
+      <c r="V19" s="3">
+        <v>-3.2803821290394275</v>
+      </c>
+      <c r="W19" s="3">
+        <v>-5.1518890610708095</v>
+      </c>
+      <c r="X19" s="3">
+        <v>-4.4191512979439915</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>-6.0569036293408214</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>-4.5118787830389486</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>-7.7472714954200228</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>-14.322113653901239</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>-13.434434222271905</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>-13.335126925724472</v>
+      </c>
+      <c r="AE19" s="3">
+        <v>-13.885284633595505</v>
+      </c>
+      <c r="AF19" s="3">
+        <v>-9.4997113884865065</v>
+      </c>
+      <c r="AG19" s="3">
+        <v>-9.3024168192941268</v>
+      </c>
+      <c r="AH19" s="3">
+        <v>-8.6365658593019727</v>
+      </c>
+      <c r="AI19" s="3">
+        <v>-12.641483061130911</v>
+      </c>
+      <c r="AJ19" s="3">
+        <v>-10.710340186357755</v>
+      </c>
+      <c r="AK19" s="3">
+        <v>-5.891064479229831</v>
+      </c>
+      <c r="AL19" s="3">
+        <v>-10.906698818870092</v>
+      </c>
+      <c r="AM19" s="3">
+        <v>-9.8618464810114492</v>
+      </c>
+      <c r="AN19" s="3">
+        <v>-35.871382896862336</v>
+      </c>
+      <c r="AO19" s="3">
+        <v>-12.168370601209453</v>
+      </c>
+      <c r="AP19" s="3">
+        <v>-10.534263125109971</v>
+      </c>
+      <c r="AQ19" s="3">
+        <v>-9.0230096996930094</v>
+      </c>
+      <c r="AR19" s="3">
+        <v>-5.5489734419628958</v>
+      </c>
+      <c r="AS19" s="3">
+        <v>-15.418808937201662</v>
+      </c>
+      <c r="AT19" s="3">
+        <v>-15.789633230545707</v>
+      </c>
+      <c r="AU19" s="3">
+        <v>-17.769620521547981</v>
+      </c>
+      <c r="AV19" s="3">
+        <v>-18.162636226759307</v>
+      </c>
+      <c r="AW19" s="3">
+        <v>-18.514134310619752</v>
+      </c>
+      <c r="AX19" s="3">
+        <v>-19.727108247945878</v>
+      </c>
+      <c r="AY19" s="3">
+        <v>-18.987546093686994</v>
+      </c>
+      <c r="AZ19" s="3">
+        <v>-24.793228424841889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>